<commit_message>
Pruebas realizadas hasta crear cliente recaudo
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/CuentasBancarias.xlsx
+++ b/MercuryTours/Resources/datapool/CuentasBancarias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14520" windowHeight="3420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="5070"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>nombre</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>1111-111005-0143</t>
+  </si>
+  <si>
+    <t>telefonia</t>
+  </si>
+  <si>
+    <t>0010-1005-222</t>
+  </si>
+  <si>
+    <t>0698.111006.1</t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +455,7 @@
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -459,8 +468,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -473,8 +485,11 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -487,8 +502,11 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -501,8 +519,11 @@
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -514,6 +535,9 @@
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>